<commit_message>
Added rating estimation of financial firms.
</commit_message>
<xml_diff>
--- a/Corporate Finance.xlsx
+++ b/Corporate Finance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18660" windowHeight="2760" tabRatio="820" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18660" windowHeight="2760" tabRatio="730" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="18" r:id="rId1"/>
@@ -41,16 +41,18 @@
     <definedName name="Beta_Regression">'Models &amp; inputs'!$F$50</definedName>
     <definedName name="Beta_Standard_Error">'Models &amp; inputs'!$F$51</definedName>
     <definedName name="Beta_Unlevered">Betas_Per_Segment[[#Totals],[Unlevered beta]]</definedName>
-    <definedName name="Company_Debt">'Company data'!$D$13</definedName>
-    <definedName name="Company_EBIT">'Company data'!$D$17</definedName>
-    <definedName name="Company_Equity">'Company data'!$D$14</definedName>
-    <definedName name="Company_Interest_Expenses">'Company data'!$D$18</definedName>
+    <definedName name="Company_Debt">'Company data'!$D$11</definedName>
+    <definedName name="Company_EBIT">'Company data'!$D$16</definedName>
+    <definedName name="Company_Equity">'Company data'!$D$12</definedName>
+    <definedName name="Company_Interest_Expenses">'Company data'!$D$17</definedName>
     <definedName name="Company_Market_Cap">'Company data'!$D$15</definedName>
-    <definedName name="Company_Tax_Rate">'Company data'!$D$88</definedName>
+    <definedName name="Company_Tax_Rate">'Company data'!$D$99</definedName>
+    <definedName name="Company_Type">'Company data'!$F$8</definedName>
     <definedName name="Confidence_interval">Investments!$E$8</definedName>
     <definedName name="Data_Validation_Regions" localSheetId="2">Regions[Regions]</definedName>
     <definedName name="Estimated_Firm_Value">Betas_Per_Segment[[#Totals],[Estimated Value]]</definedName>
-    <definedName name="Industry_Average">'Company data'!$C$51</definedName>
+    <definedName name="Industry_Average">'Company data'!$C$62</definedName>
+    <definedName name="Input_Company_Types">Company_Types[Type of company]</definedName>
     <definedName name="Input_Confidence_Interval" localSheetId="5">Confidence_Intervals[Confidence intervals]</definedName>
     <definedName name="Input_Confidence_Interval">Confidence_Intervals[Confidence intervals]</definedName>
     <definedName name="Input_Industries" localSheetId="5">Industries[Industries]</definedName>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2794" uniqueCount="528">
   <si>
     <t>S&amp;P</t>
   </si>
@@ -1513,9 +1515,6 @@
     <t>Estimated debt</t>
   </si>
   <si>
-    <t>Strange debt allocator</t>
-  </si>
-  <si>
     <t>Allocated debt</t>
   </si>
   <si>
@@ -1534,9 +1533,6 @@
     <t>Firm value proportion * Levered Beta debt</t>
   </si>
   <si>
-    <t>Internet coverage ratio is</t>
-  </si>
-  <si>
     <t>&gt;</t>
   </si>
   <si>
@@ -1586,18 +1582,94 @@
   </si>
   <si>
     <t>Market cap</t>
+  </si>
+  <si>
+    <t>Special thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To </t>
+  </si>
+  <si>
+    <t>To Prof. Aswath Damodran at NYU for collecting and providing the data used for calculations and estimations.</t>
+  </si>
+  <si>
+    <t>Large manufactuing firms</t>
+  </si>
+  <si>
+    <t>For smaller firms</t>
+  </si>
+  <si>
+    <t>greater than</t>
+  </si>
+  <si>
+    <t>Rating is</t>
+  </si>
+  <si>
+    <t>Financial service firms</t>
+  </si>
+  <si>
+    <t>Rental leases or rental commitments</t>
+  </si>
+  <si>
+    <t>Long term government bond rate</t>
+  </si>
+  <si>
+    <t>Estimated cost per debt</t>
+  </si>
+  <si>
+    <t>Estimated default spread</t>
+  </si>
+  <si>
+    <t>Strange debt allocator constant</t>
+  </si>
+  <si>
+    <t>Cost of debt</t>
+  </si>
+  <si>
+    <t>Things that could be added</t>
+  </si>
+  <si>
+    <t>Operational leases from ratings book.</t>
+  </si>
+  <si>
+    <t>Synthetic ratings</t>
+  </si>
+  <si>
+    <t>Type of company</t>
+  </si>
+  <si>
+    <t>Small risky firm</t>
+  </si>
+  <si>
+    <t>Large manufacturing firm</t>
+  </si>
+  <si>
+    <t>Rating table</t>
+  </si>
+  <si>
+    <t>Rating_Large_Firms</t>
+  </si>
+  <si>
+    <t>Rating_Small_Firms</t>
+  </si>
+  <si>
+    <t>Rating_Financial_Firms</t>
+  </si>
+  <si>
+    <t>Financial service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0000%"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -2257,7 +2329,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2276,8 +2348,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -2608,6 +2681,18 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" xfId="9" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="18" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2675,11 +2760,8 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" xfId="9" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Beräkning" xfId="9" builtinId="22"/>
     <cellStyle name="Hyperlänk" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlänk 2" xfId="7"/>
@@ -2695,6 +2777,7 @@
     <cellStyle name="Tusental 2" xfId="5"/>
     <cellStyle name="Utdata" xfId="10" builtinId="21"/>
     <cellStyle name="Valuta 2" xfId="6"/>
+    <cellStyle name="Valuta 3" xfId="15"/>
   </cellStyles>
   <dxfs count="184">
     <dxf>
@@ -5825,11 +5908,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Betas_Per_Segment" displayName="Betas_Per_Segment" ref="C53:Q61" totalsRowCount="1" totalsRowDxfId="182" tableBorderDxfId="183" headerRowCellStyle="Normal" totalsRowCellStyle="Normal">
-  <autoFilter ref="C53:Q60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Betas_Per_Segment" displayName="Betas_Per_Segment" ref="C64:Q72" totalsRowCount="1" totalsRowDxfId="182" tableBorderDxfId="183" headerRowCellStyle="Normal" totalsRowCellStyle="Normal">
+  <autoFilter ref="C64:Q71"/>
   <tableColumns count="15">
     <tableColumn id="7" name="Segment" totalsRowLabel="Company" dataDxfId="181" totalsRowDxfId="180" dataCellStyle="Länkad cell">
-      <calculatedColumnFormula>IF(C40="","",C40)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(C51="","",C51)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" name="EV/Sales" dataDxfId="179" totalsRowDxfId="178" dataCellStyle="Beräkning">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</calculatedColumnFormula>
@@ -5855,7 +5938,7 @@
       <calculatedColumnFormula>IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Estimated debt" dataDxfId="169" totalsRowDxfId="168" dataCellStyle="Utdata">
-      <calculatedColumnFormula>IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" name="Estimated equity" dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Utdata">
       <calculatedColumnFormula>IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</calculatedColumnFormula>
@@ -6072,8 +6155,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Company_Operations_Region" displayName="Company_Operations_Region" ref="C24:D34" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="C24:D34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Company_Operations_Region" displayName="Company_Operations_Region" ref="C35:D45" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="C35:D45"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Region" dataCellStyle="Normal"/>
     <tableColumn id="2" name="Percentage" dataDxfId="159" dataCellStyle="Indata"/>
@@ -6156,6 +6239,22 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Rating_Financial_Firms" displayName="Rating_Financial_Firms" ref="N142:Q157" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="N142:Q157"/>
+  <sortState ref="N143:Q157">
+    <sortCondition descending="1" ref="O142:O157"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="greater than" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="&lt;= to" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Rating is" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Spread is" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Regions" displayName="Regions" ref="B7:C17" totalsRowShown="0">
   <autoFilter ref="B7:C17"/>
   <sortState ref="B8:B17">
@@ -6169,7 +6268,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="User_answers" displayName="User_answers" ref="E7:E9" totalsRowShown="0">
   <autoFilter ref="E7:E9"/>
   <tableColumns count="1">
@@ -6179,7 +6278,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Confidence_Intervals" displayName="Confidence_Intervals" ref="E11:E13" totalsRowShown="0" dataCellStyle="Procent">
   <autoFilter ref="E11:E13"/>
   <tableColumns count="1">
@@ -6189,7 +6288,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Industries" displayName="Industries" ref="G7:G89" totalsRowShown="0" dataCellStyle="Normal 3">
   <autoFilter ref="G7:G89"/>
   <tableColumns count="1">
@@ -6199,7 +6298,42 @@
 </table>
 </file>
 
-<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Betas_Per_Segment_Region" displayName="Betas_Per_Segment_Region" ref="C75:L83" totalsRowCount="1" tableBorderDxfId="158">
+  <autoFilter ref="C75:L82"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Segment" totalsRowLabel="Company" dataDxfId="157" totalsRowDxfId="156"/>
+    <tableColumn id="18" name="EV/Sales" dataDxfId="155" dataCellStyle="Beräkning">
+      <calculatedColumnFormula>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" name="Estimated Value" totalsRowFunction="custom" dataDxfId="154" dataCellStyle="Beräkning">
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Betas_Per_Segment_Region[Estimated Value])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="20" name="Firm Value Proportion" dataCellStyle="Beräkning">
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="Unlevered beta" totalsRowFunction="custom" dataDxfId="153" totalsRowDxfId="152" dataCellStyle="Utdata">
+      <totalsRowFormula>SUM(Betas_Per_Segment_Region[Firm value proportion * Unlevered Beta])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="16" name="Firm value proportion * Unlevered Beta" dataDxfId="151" dataCellStyle="Beräkning">
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" name="Estimated levered beta" totalsRowFunction="custom" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Utdata">
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Betas_Per_Segment_Region[Firm value proportion * Levered Beta])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="22" name="Estimated levered beta using debt allocation" dataCellStyle="Utdata"/>
+    <tableColumn id="23" name="Industry D/E" dataCellStyle="Utdata"/>
+    <tableColumn id="21" name="Firm value proportion * Levered Beta" dataDxfId="148" dataCellStyle="Beräkning">
+      <calculatedColumnFormula>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Industry_TableConverter" displayName="Industry_TableConverter" ref="B19:D25" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="B19:D25"/>
   <tableColumns count="3">
@@ -6211,44 +6345,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tabell28" displayName="Tabell28" ref="C64:L72" totalsRowCount="1" tableBorderDxfId="158">
-  <autoFilter ref="C64:L71"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Segment" totalsRowLabel="Company" dataDxfId="157" totalsRowDxfId="156"/>
-    <tableColumn id="18" name="EV/Sales" dataDxfId="155" dataCellStyle="Beräkning">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="19" name="Estimated Value" totalsRowFunction="custom" dataDxfId="154" dataCellStyle="Beräkning">
-      <calculatedColumnFormula>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabell28[Estimated Value])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="20" name="Firm Value Proportion" dataCellStyle="Beräkning">
-      <calculatedColumnFormula>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" name="Unlevered beta" totalsRowFunction="custom" dataDxfId="153" totalsRowDxfId="152" dataCellStyle="Utdata">
-      <totalsRowFormula>SUM(Tabell28[Firm value proportion * Unlevered Beta])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="16" name="Firm value proportion * Unlevered Beta" dataDxfId="151" dataCellStyle="Beräkning">
-      <calculatedColumnFormula>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="17" name="Estimated levered beta" totalsRowFunction="custom" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Utdata">
-      <calculatedColumnFormula>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabell28[Firm value proportion * Levered Beta])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="22" name="Estimated levered beta using debt allocation" dataCellStyle="Utdata"/>
-    <tableColumn id="23" name="Industry D/E" dataCellStyle="Utdata"/>
-    <tableColumn id="21" name="Firm value proportion * Levered Beta" dataDxfId="148" dataCellStyle="Beräkning">
-      <calculatedColumnFormula>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</calculatedColumnFormula>
-    </tableColumn>
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Company_Types" displayName="Company_Types" ref="I7:J10" totalsRowShown="0">
+  <autoFilter ref="I7:J10"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Type of company"/>
+    <tableColumn id="2" name="Rating table"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Operations_Per_Segment_Region" displayName="Operations_Per_Segment_Region" ref="C39:J47" totalsRowShown="0" tableBorderDxfId="147">
-  <autoFilter ref="C39:J47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Operations_Per_Segment_Region" displayName="Operations_Per_Segment_Region" ref="C50:J58" totalsRowShown="0" tableBorderDxfId="147">
+  <autoFilter ref="C50:J58"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Segment" dataDxfId="146" dataCellStyle="Indata"/>
     <tableColumn id="2" name="Revenue" dataDxfId="145" dataCellStyle="Indata"/>
@@ -6648,12 +6758,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -6676,7 +6786,7 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="2:14" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
@@ -6699,10 +6809,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad5"/>
-  <dimension ref="B1:N76"/>
+  <dimension ref="B1:N81"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E10:E16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6722,12 +6832,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -6750,7 +6860,7 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="2:14" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
@@ -6769,48 +6879,95 @@
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="169" t="s">
         <v>464</v>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="165" t="s">
+      <c r="B11" s="169" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="165"/>
-      <c r="D11" s="165"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="169" t="s">
         <v>465</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="169" t="s">
         <v>466</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="169"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="169" t="s">
         <v>462</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="169" t="s">
         <v>468</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-    </row>
-    <row r="76" ht="30.75" customHeight="1"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="169"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="165" t="s">
+        <v>519</v>
+      </c>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="165"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="165"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="165"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="165"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="165" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="164" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="164" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="81" ht="30.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B14:D14"/>
@@ -6833,10 +6990,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X126"/>
+  <dimension ref="B1:X137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6863,12 +7020,12 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="2:15" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="C2" s="164" t="s">
+      <c r="C2" s="168" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="3" spans="2:15" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="C3" s="164"/>
+      <c r="C3" s="168"/>
       <c r="D3" s="23"/>
       <c r="E3" s="25" t="s">
         <v>206</v>
@@ -6890,7 +7047,7 @@
       <c r="O3" s="22"/>
     </row>
     <row r="4" spans="2:15" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="C4" s="164"/>
+      <c r="C4" s="168"/>
     </row>
     <row r="5" spans="2:15" ht="7.5" customHeight="1">
       <c r="C5" s="1"/>
@@ -6899,1310 +7056,1383 @@
       <c r="B7" t="s">
         <v>271</v>
       </c>
+      <c r="F7" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="8" spans="2:15">
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
+      <c r="C8" s="174"/>
+      <c r="D8" s="174"/>
+      <c r="F8" s="48" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="C11" s="132" t="s">
+        <v>450</v>
+      </c>
+      <c r="D11" s="48">
+        <v>7500</v>
+      </c>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
-      <c r="C13" s="132" t="s">
-        <v>450</v>
-      </c>
-      <c r="D13" s="48">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15">
-      <c r="C14" s="163" t="s">
+      <c r="C12" s="163" t="s">
         <v>451</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D12" s="48">
         <v>10000</v>
       </c>
-      <c r="E14" s="136" t="s">
+      <c r="E12" s="136" t="s">
         <v>453</v>
       </c>
-      <c r="F14" s="137">
+      <c r="F12" s="137">
         <f>Company_Debt/Company_Equity</f>
         <v>0.75</v>
       </c>
     </row>
+    <row r="13" spans="2:15">
+      <c r="E13" s="136"/>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="E14" s="136"/>
+    </row>
     <row r="15" spans="2:15">
+      <c r="B15" s="136"/>
       <c r="C15" s="163" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D15" s="48">
-        <v>0</v>
+        <v>10000000000</v>
       </c>
       <c r="E15" s="136"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" s="136"/>
-      <c r="C16" s="136"/>
-      <c r="D16" s="136"/>
+      <c r="C16" s="132" t="s">
+        <v>498</v>
+      </c>
+      <c r="D16" s="162">
+        <v>1000</v>
+      </c>
       <c r="E16" s="136"/>
       <c r="F16" s="136"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="136"/>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="136" t="s">
+        <v>499</v>
+      </c>
+      <c r="D17" s="162">
         <v>500</v>
       </c>
-      <c r="D17" s="162">
-        <v>1000</v>
-      </c>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
+      <c r="E17" s="136" t="s">
+        <v>500</v>
+      </c>
+      <c r="F17" s="154">
+        <f>IFERROR(Company_EBIT/Company_Interest_Expenses,"")</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="136"/>
-      <c r="C18" s="136" t="s">
+      <c r="C18" s="132" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="136" t="s">
         <v>501</v>
       </c>
-      <c r="D18" s="162">
-        <v>210</v>
-      </c>
-      <c r="E18" s="136" t="s">
-        <v>502</v>
-      </c>
-      <c r="F18" s="154">
-        <f>IFERROR(Company_EBIT/Company_Interest_Expenses,"")</f>
-        <v>4.7619047619047619</v>
+      <c r="F18" s="166" t="str">
+        <f ca="1">INDEX(INDIRECT(VLOOKUP(Company_Type,Company_Types[],2,FALSE)),MATCH(F17,INDIRECT(CONCATENATE(VLOOKUP(Company_Type,Company_Types[],2,FALSE),"[&lt;= to]")),-1),3)</f>
+        <v>B</v>
+      </c>
+      <c r="G18" s="166" t="str">
+        <f ca="1">INDEX(INDIRECT(VLOOKUP(Company_Type,Company_Types[],2,FALSE)),MATCH(F17,INDIRECT(CONCATENATE(VLOOKUP(Company_Type,Company_Types[],2,FALSE),"[&lt;= to]")),-1),4)</f>
+        <v>B2</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="C19" s="132"/>
+      <c r="B19" s="136"/>
+      <c r="E19" t="s">
+        <v>514</v>
+      </c>
+      <c r="F19" s="167">
+        <f>IF(Company_Market_Cap&gt;5000000000,INDEX(Rating_Large_Firms[],MATCH(F17,Rating_Large_Firms[&lt;= to],-1),5),INDEX(Rating_Small_Firms[],MATCH(F17,Rating_Small_Firms[&lt;= to],-1),5))</f>
+        <v>0.04</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="C20" s="132" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="136" t="s">
-        <v>503</v>
-      </c>
-      <c r="F20" s="187" t="str">
-        <f>IF(Company_Market_Cap&gt;5000000000,INDEX(Rating_Large_Firms[],MATCH(F18,Rating_Large_Firms[&lt;= to],-1),3),INDEX(Rating_Small_Firms[],MATCH(F18,Rating_Small_Firms[&lt;= to],-1),3))</f>
-        <v>A-</v>
-      </c>
-      <c r="G20" s="187" t="str">
-        <f>IF(Company_Market_Cap&gt;5000000000,INDEX(Rating_Large_Firms[],MATCH(F18,Rating_Large_Firms[&lt;= to],-1),4),INDEX(Rating_Small_Firms[],MATCH(F18,Rating_Small_Firms[&lt;= to],-1),4))</f>
-        <v>A3</v>
-      </c>
+      <c r="B20" s="136"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="C21" s="132"/>
+      <c r="B21" s="136"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="C22" s="132"/>
+      <c r="B22" s="136"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" t="s">
+      <c r="B23" s="136"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="136"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="136"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="136"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="136"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="136"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="136"/>
+    </row>
+    <row r="30" spans="2:7" ht="30">
+      <c r="B30" s="136"/>
+      <c r="C30" s="53" t="s">
+        <v>511</v>
+      </c>
+      <c r="D30" s="162"/>
+    </row>
+    <row r="31" spans="2:7" ht="30">
+      <c r="B31" s="136"/>
+      <c r="C31" s="53" t="s">
+        <v>512</v>
+      </c>
+      <c r="D31" s="162"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="136"/>
+      <c r="C32" s="136" t="s">
+        <v>516</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="127" t="s">
+        <v>513</v>
+      </c>
+      <c r="F32" s="138">
+        <f>D31+F19</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="C33" s="132"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
         <v>256</v>
       </c>
-      <c r="E23" s="136"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="C24" t="s">
+      <c r="E34" s="136"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="C35" t="s">
         <v>202</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D35" t="s">
         <v>413</v>
       </c>
-      <c r="E24" s="136"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="C25" t="s">
+      <c r="E35" s="136"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" t="s">
         <v>232</v>
       </c>
-      <c r="D25" s="135">
+      <c r="D36" s="135">
         <v>0.12</v>
       </c>
-      <c r="E25" s="136"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="C26" t="s">
+      <c r="E36" s="136"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="C37" t="s">
         <v>238</v>
       </c>
-      <c r="D26" s="135">
+      <c r="D37" s="135">
         <v>0.25</v>
       </c>
-      <c r="E26" s="136"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="C27" t="s">
+      <c r="E37" s="136"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="C38" t="s">
         <v>237</v>
       </c>
-      <c r="D27" s="135">
+      <c r="D38" s="135">
         <v>0.13</v>
       </c>
-      <c r="E27" s="136"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="C28" t="s">
+      <c r="E38" s="136"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="C39" t="s">
         <v>233</v>
       </c>
-      <c r="D28" s="135">
+      <c r="D39" s="135">
         <v>0.05</v>
       </c>
-      <c r="E28" s="136"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="C29" t="s">
+      <c r="E39" s="136"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="C40" t="s">
         <v>235</v>
       </c>
-      <c r="D29" s="135">
+      <c r="D40" s="135">
         <v>0.04</v>
       </c>
-      <c r="E29" s="136"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="C30" t="s">
+      <c r="E40" s="136"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="C41" t="s">
         <v>236</v>
       </c>
-      <c r="D30" s="135">
+      <c r="D41" s="135">
         <v>0</v>
       </c>
-      <c r="E30" s="136"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="C31" t="s">
+      <c r="E41" s="136"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="C42" t="s">
         <v>242</v>
       </c>
-      <c r="D31" s="135">
+      <c r="D42" s="135">
         <v>0.08</v>
       </c>
-      <c r="E31" s="136"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="C32" t="s">
+      <c r="E42" s="136"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="C43" t="s">
         <v>240</v>
       </c>
-      <c r="D32" s="135">
+      <c r="D43" s="135">
         <v>0.33</v>
       </c>
-      <c r="E32" s="136"/>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="C33" t="s">
+      <c r="E43" s="136"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="C44" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="135">
+      <c r="D44" s="135">
         <v>0</v>
       </c>
-      <c r="E33" s="136"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1">
-      <c r="C34" t="s">
+      <c r="E44" s="136"/>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1">
+      <c r="C45" t="s">
         <v>239</v>
       </c>
-      <c r="D34" s="135">
+      <c r="D45" s="135">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C35" s="47" t="s">
+    <row r="46" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C46" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="D35" s="44">
-        <f>SUM(D25:D34)</f>
+      <c r="D46" s="44">
+        <f>SUM(D36:D45)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15.75" thickTop="1">
-      <c r="C36" s="47"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" t="s">
+    <row r="47" spans="2:5" ht="15.75" thickTop="1">
+      <c r="C47" s="47"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" t="s">
         <v>470</v>
       </c>
-      <c r="C37" s="47"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1">
-      <c r="C38" s="47"/>
-      <c r="E38" s="167" t="s">
+      <c r="C48" s="47"/>
+    </row>
+    <row r="49" spans="2:19" ht="15.75" thickBot="1">
+      <c r="C49" s="47"/>
+      <c r="E49" s="171" t="s">
         <v>472</v>
       </c>
-      <c r="F38" s="167"/>
-      <c r="G38" s="167"/>
-      <c r="H38" s="167"/>
-      <c r="I38" s="167"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1">
-      <c r="C39" t="s">
+      <c r="F49" s="171"/>
+      <c r="G49" s="171"/>
+      <c r="H49" s="171"/>
+      <c r="I49" s="171"/>
+    </row>
+    <row r="50" spans="2:19" ht="15.75" thickBot="1">
+      <c r="C50" t="s">
         <v>469</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D50" t="s">
         <v>471</v>
       </c>
-      <c r="E39" s="145" t="s">
+      <c r="E50" s="145" t="s">
         <v>420</v>
       </c>
-      <c r="F39" s="145" t="s">
+      <c r="F50" s="145" t="s">
         <v>282</v>
       </c>
-      <c r="G39" s="145" t="s">
+      <c r="G50" s="145" t="s">
         <v>415</v>
       </c>
-      <c r="H39" s="145" t="s">
+      <c r="H50" s="145" t="s">
         <v>283</v>
       </c>
-      <c r="I39" s="145" t="s">
+      <c r="I50" s="145" t="s">
         <v>408</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J50" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C40" s="114" t="s">
+    <row r="51" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C51" s="114" t="s">
         <v>360</v>
       </c>
-      <c r="D40" s="115">
+      <c r="D51" s="115">
         <v>40000</v>
       </c>
-      <c r="E40" s="133">
+      <c r="E51" s="133">
         <v>0.5</v>
       </c>
-      <c r="F40" s="133"/>
-      <c r="G40" s="133">
+      <c r="F51" s="133"/>
+      <c r="G51" s="133">
         <v>0.5</v>
       </c>
-      <c r="H40" s="133"/>
-      <c r="I40" s="133"/>
-      <c r="J40" s="149">
+      <c r="H51" s="133"/>
+      <c r="I51" s="133"/>
+      <c r="J51" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C41" s="114" t="s">
+    <row r="52" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C52" s="114" t="s">
         <v>323</v>
       </c>
-      <c r="D41" s="115">
+      <c r="D52" s="115">
         <v>10000</v>
       </c>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="149">
+      <c r="E52" s="133"/>
+      <c r="F52" s="133"/>
+      <c r="G52" s="133"/>
+      <c r="H52" s="133"/>
+      <c r="I52" s="133"/>
+      <c r="J52" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C42" s="114" t="s">
+    <row r="53" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C53" s="114" t="s">
         <v>325</v>
       </c>
-      <c r="D42" s="115">
+      <c r="D53" s="115">
         <v>8000</v>
       </c>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="133"/>
-      <c r="I42" s="133"/>
-      <c r="J42" s="149">
+      <c r="E53" s="133"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="133"/>
+      <c r="I53" s="133"/>
+      <c r="J53" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="133"/>
-      <c r="H43" s="133"/>
-      <c r="I43" s="133"/>
-      <c r="J43" s="149">
+    <row r="54" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C54" s="114"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="133"/>
+      <c r="F54" s="133"/>
+      <c r="G54" s="133"/>
+      <c r="H54" s="133"/>
+      <c r="I54" s="133"/>
+      <c r="J54" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C44" s="114"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="133"/>
-      <c r="F44" s="133"/>
-      <c r="G44" s="133"/>
-      <c r="H44" s="133"/>
-      <c r="I44" s="133"/>
-      <c r="J44" s="149">
+    <row r="55" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C55" s="114"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="133"/>
+      <c r="F55" s="133"/>
+      <c r="G55" s="133"/>
+      <c r="H55" s="133"/>
+      <c r="I55" s="133"/>
+      <c r="J55" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C45" s="116"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="133"/>
-      <c r="F45" s="133"/>
-      <c r="G45" s="133"/>
-      <c r="H45" s="133"/>
-      <c r="I45" s="133"/>
-      <c r="J45" s="149">
+    <row r="56" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C56" s="116"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="133"/>
+      <c r="F56" s="133"/>
+      <c r="G56" s="133"/>
+      <c r="H56" s="133"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C46" s="114"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="133"/>
-      <c r="F46" s="133"/>
-      <c r="G46" s="133"/>
-      <c r="H46" s="133"/>
-      <c r="I46" s="133"/>
-      <c r="J46" s="149">
+    <row r="57" spans="2:19" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C57" s="114"/>
+      <c r="D57" s="114"/>
+      <c r="E57" s="133"/>
+      <c r="F57" s="133"/>
+      <c r="G57" s="133"/>
+      <c r="H57" s="133"/>
+      <c r="I57" s="133"/>
+      <c r="J57" s="149">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:10" ht="15.75" thickTop="1">
-      <c r="C47" s="146" t="s">
+    <row r="58" spans="2:19" ht="15.75" thickTop="1">
+      <c r="C58" s="146" t="s">
         <v>302</v>
       </c>
-      <c r="D47" s="147">
-        <f>SUM(D40:D46)</f>
+      <c r="D58" s="147">
+        <f>SUM(D51:D57)</f>
         <v>58000</v>
       </c>
-      <c r="J47">
+      <c r="J58">
         <f>SUM(Operations_Per_Segment_Region[[#This Row],[US]:[Emerging markets]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:24">
-      <c r="B49" t="str">
+    <row r="60" spans="2:19">
+      <c r="B60" t="str">
         <f>CONCATENATE("Betas for each business segment (using ",Industry_Average," for industry averages)")</f>
         <v>Betas for each business segment (using US for industry averages)</v>
       </c>
     </row>
-    <row r="50" spans="2:24">
-      <c r="C50" t="s">
+    <row r="61" spans="2:19">
+      <c r="C61" t="s">
         <v>475</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F61" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19">
+      <c r="C62" s="172" t="s">
+        <v>420</v>
+      </c>
+      <c r="D62" s="173"/>
+      <c r="F62" s="48">
+        <v>1.3871</v>
+      </c>
+      <c r="L62" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19">
+      <c r="H63" t="s">
+        <v>476</v>
+      </c>
+      <c r="I63" s="113"/>
+      <c r="N63" t="s">
+        <v>430</v>
+      </c>
+      <c r="O63" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="64" spans="2:19" ht="29.25" customHeight="1">
+      <c r="C64" s="157" t="s">
+        <v>469</v>
+      </c>
+      <c r="D64" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="E64" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="F64" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="G64" s="157" t="s">
+        <v>301</v>
+      </c>
+      <c r="H64" s="157" t="s">
+        <v>443</v>
+      </c>
+      <c r="I64" s="157" t="s">
+        <v>457</v>
+      </c>
+      <c r="J64" s="157" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="51" spans="2:24">
-      <c r="C51" s="168" t="s">
-        <v>420</v>
-      </c>
-      <c r="D51" s="169"/>
-      <c r="F51" s="48">
-        <v>1.3871</v>
-      </c>
-      <c r="L51" t="s">
+      <c r="K64" s="157" t="s">
+        <v>479</v>
+      </c>
+      <c r="L64" s="157" t="s">
+        <v>481</v>
+      </c>
+      <c r="M64" s="157" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="52" spans="2:24">
-      <c r="H52" t="s">
-        <v>476</v>
-      </c>
-      <c r="I52" s="113"/>
-      <c r="N52" t="s">
-        <v>430</v>
-      </c>
-      <c r="O52" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="53" spans="2:24" ht="29.25" customHeight="1">
-      <c r="C53" s="157" t="s">
-        <v>469</v>
-      </c>
-      <c r="D53" s="40" t="s">
-        <v>298</v>
-      </c>
-      <c r="E53" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="F53" s="40" t="s">
-        <v>300</v>
-      </c>
-      <c r="G53" s="157" t="s">
-        <v>301</v>
-      </c>
-      <c r="H53" s="157" t="s">
-        <v>443</v>
-      </c>
-      <c r="I53" s="157" t="s">
-        <v>457</v>
-      </c>
-      <c r="J53" s="157" t="s">
-        <v>481</v>
-      </c>
-      <c r="K53" s="157" t="s">
-        <v>479</v>
-      </c>
-      <c r="L53" s="157" t="s">
-        <v>482</v>
-      </c>
-      <c r="M53" s="157" t="s">
+      <c r="N64" s="157" t="s">
+        <v>477</v>
+      </c>
+      <c r="O64" s="159" t="s">
+        <v>478</v>
+      </c>
+      <c r="P64" s="159" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q64" s="73" t="s">
         <v>484</v>
       </c>
-      <c r="N53" s="157" t="s">
-        <v>477</v>
-      </c>
-      <c r="O53" s="159" t="s">
-        <v>478</v>
-      </c>
-      <c r="P53" s="159" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q53" s="73" t="s">
-        <v>485</v>
-      </c>
-      <c r="S53" s="79"/>
-    </row>
-    <row r="54" spans="2:24" ht="15" customHeight="1" thickBot="1">
-      <c r="C54" s="148" t="str">
-        <f t="shared" ref="C54:C60" si="0">IF(C40="","",C40)</f>
+      <c r="S64" s="79"/>
+    </row>
+    <row r="65" spans="2:24" ht="15" customHeight="1" thickBot="1">
+      <c r="C65" s="148" t="str">
+        <f t="shared" ref="C65:C71" si="0">IF(C51="","",C51)</f>
         <v>Metals &amp; Mining</v>
       </c>
-      <c r="D54" s="154">
+      <c r="D65" s="154">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v>3.6008672528701777</v>
       </c>
-      <c r="E54" s="72">
+      <c r="E65" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v>144034.6901148071</v>
       </c>
-      <c r="F54" s="138">
+      <c r="F65" s="138">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v>0.82498375495636911</v>
       </c>
-      <c r="G54" s="125">
+      <c r="G65" s="125">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v>0.90451447164101273</v>
       </c>
-      <c r="H54" s="72">
+      <c r="H65" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>0.74620974522677896</v>
       </c>
-      <c r="I54" s="152">
+      <c r="I65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>1.3454652765660065</v>
       </c>
-      <c r="J54" s="152">
+      <c r="J65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v>5983.1411278702999</v>
       </c>
-      <c r="K54" s="152">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
+      <c r="K65" s="152">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
         <v>50064.218996829528</v>
       </c>
-      <c r="L54" s="152">
+      <c r="L65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v>138051.5489869368</v>
       </c>
-      <c r="M54" s="152">
+      <c r="M65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v>8262.0606559176176</v>
       </c>
-      <c r="N54" s="152">
+      <c r="N65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v>1.3302792626437849</v>
       </c>
-      <c r="O54" s="152">
+      <c r="O65" s="152">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v>0.48213439495131194</v>
       </c>
-      <c r="P54" s="152">
+      <c r="P65" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v>1.0974587812364596</v>
       </c>
-      <c r="Q54" s="72">
+      <c r="Q65" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>1.1099869960248336</v>
       </c>
-      <c r="R54" s="171" t="s">
+      <c r="R65" s="175" t="s">
         <v>456</v>
       </c>
-      <c r="S54" s="171"/>
-      <c r="T54" s="171"/>
-    </row>
-    <row r="55" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C55" s="148" t="str">
+      <c r="S65" s="175"/>
+      <c r="T65" s="175"/>
+    </row>
+    <row r="66" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C66" s="148" t="str">
         <f t="shared" si="0"/>
         <v>Chemical (Diversified)</v>
       </c>
-      <c r="D55" s="154">
+      <c r="D66" s="154">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v>1.6650619259181105</v>
       </c>
-      <c r="E55" s="72">
+      <c r="E66" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v>16650.619259181105</v>
       </c>
-      <c r="F55" s="138">
+      <c r="F66" s="138">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v>9.5369319625980303E-2</v>
       </c>
-      <c r="G55" s="125">
+      <c r="G66" s="125">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v>1.2160388085910969</v>
       </c>
-      <c r="H55" s="72">
+      <c r="H66" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>0.11597279381412061</v>
       </c>
-      <c r="I55" s="153">
+      <c r="I66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>1.8088577277792568</v>
       </c>
-      <c r="J55" s="153">
+      <c r="J66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v>478.99696683019607</v>
       </c>
-      <c r="K55" s="153">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
+      <c r="K66" s="153">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
         <v>4008.0299852027606</v>
       </c>
-      <c r="L55" s="153">
+      <c r="L66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v>16171.622292350909</v>
       </c>
-      <c r="M55" s="153">
+      <c r="M66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v>967.83357567857308</v>
       </c>
-      <c r="N55" s="153">
+      <c r="N66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v>1.607233426214749</v>
       </c>
-      <c r="O55" s="153">
+      <c r="O66" s="153">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v>0.33389379133206926</v>
       </c>
-      <c r="P55" s="153">
+      <c r="P66" s="153">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v>0.15328075833823382</v>
       </c>
-      <c r="Q55" s="72">
+      <c r="Q66" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>0.17250953079850442</v>
       </c>
-      <c r="R55" s="171"/>
-      <c r="S55" s="171"/>
-      <c r="T55" s="171"/>
-    </row>
-    <row r="56" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C56" s="148" t="str">
+      <c r="R66" s="175"/>
+      <c r="S66" s="175"/>
+      <c r="T66" s="175"/>
+    </row>
+    <row r="67" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C67" s="148" t="str">
         <f t="shared" si="0"/>
         <v>Coal &amp; Related Energy</v>
       </c>
-      <c r="D56" s="154">
+      <c r="D67" s="154">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v>1.7382039573820396</v>
       </c>
-      <c r="E56" s="72">
+      <c r="E67" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v>13905.631659056316</v>
       </c>
-      <c r="F56" s="138">
+      <c r="F67" s="138">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v>7.9646925417650505E-2</v>
       </c>
-      <c r="G56" s="125">
+      <c r="G67" s="125">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v>0.73477287574552486</v>
       </c>
-      <c r="H56" s="72">
+      <c r="H67" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>5.8522400433416402E-2</v>
       </c>
-      <c r="I56" s="152">
+      <c r="I67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>1.0929746526714683</v>
       </c>
-      <c r="J56" s="152">
+      <c r="J67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v>1037.8619052995036</v>
       </c>
-      <c r="K56" s="152">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
+      <c r="K67" s="152">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
         <v>8684.3590356485838</v>
       </c>
-      <c r="L56" s="152">
+      <c r="L67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v>12867.769753756813</v>
       </c>
-      <c r="M56" s="152">
+      <c r="M67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v>770.10576840380793</v>
       </c>
-      <c r="N56" s="152">
+      <c r="N67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v>1.3784316110083095</v>
       </c>
-      <c r="O56" s="152">
+      <c r="O67" s="152">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v>0.86627308371877576</v>
       </c>
-      <c r="P56" s="152">
+      <c r="P67" s="152">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v>0.10978783971531066</v>
       </c>
-      <c r="Q56" s="72">
+      <c r="Q67" s="72">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v>8.7052070644706908E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C57" s="148" t="str">
+    <row r="68" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C68" s="148" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D57" s="154" t="str">
+      <c r="D68" s="154" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E57" s="72" t="str">
+      <c r="E68" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F57" s="138" t="str">
+      <c r="F68" s="138" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v/>
       </c>
-      <c r="G57" s="125" t="str">
+      <c r="G68" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H57" s="72" t="str">
+      <c r="H68" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="I57" s="152" t="str">
+      <c r="I68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v/>
       </c>
-      <c r="J57" s="152" t="str">
+      <c r="J68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v/>
       </c>
-      <c r="K57" s="152" t="str">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
-        <v/>
-      </c>
-      <c r="L57" s="152" t="str">
+      <c r="K68" s="152" t="str">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
+        <v/>
+      </c>
+      <c r="L68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v/>
       </c>
-      <c r="M57" s="152" t="str">
+      <c r="M68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v/>
       </c>
-      <c r="N57" s="152" t="str">
+      <c r="N68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v/>
       </c>
-      <c r="O57" s="152" t="str">
+      <c r="O68" s="152" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="P57" s="152" t="str">
+      <c r="P68" s="152" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v/>
       </c>
-      <c r="Q57" s="72" t="str">
+      <c r="Q68" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="S57" t="s">
+      <c r="S68" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="58" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C58" s="148" t="str">
+    <row r="69" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C69" s="148" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D58" s="154" t="str">
+      <c r="D69" s="154" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E58" s="72" t="str">
+      <c r="E69" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F58" s="138" t="str">
+      <c r="F69" s="138" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v/>
       </c>
-      <c r="G58" s="125" t="str">
+      <c r="G69" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H58" s="72" t="str">
+      <c r="H69" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="I58" s="125" t="str">
+      <c r="I69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v/>
       </c>
-      <c r="J58" s="125" t="str">
+      <c r="J69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v/>
       </c>
-      <c r="K58" s="125" t="str">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
-        <v/>
-      </c>
-      <c r="L58" s="125" t="str">
+      <c r="K69" s="125" t="str">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
+        <v/>
+      </c>
+      <c r="L69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v/>
       </c>
-      <c r="M58" s="125" t="str">
+      <c r="M69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v/>
       </c>
-      <c r="N58" s="125" t="str">
+      <c r="N69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v/>
       </c>
-      <c r="O58" s="125" t="str">
+      <c r="O69" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="P58" s="125" t="str">
+      <c r="P69" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v/>
       </c>
-      <c r="Q58" s="72" t="str">
+      <c r="Q69" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C59" s="148" t="str">
+    <row r="70" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C70" s="148" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D59" s="154" t="str">
+      <c r="D70" s="154" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E59" s="74" t="str">
+      <c r="E70" s="74" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F59" s="139" t="str">
+      <c r="F70" s="139" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v/>
       </c>
-      <c r="G59" s="125" t="str">
+      <c r="G70" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H59" s="72" t="str">
+      <c r="H70" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="I59" s="125" t="str">
+      <c r="I70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v/>
       </c>
-      <c r="J59" s="125" t="str">
+      <c r="J70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v/>
       </c>
-      <c r="K59" s="125" t="str">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
-        <v/>
-      </c>
-      <c r="L59" s="125" t="str">
+      <c r="K70" s="125" t="str">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
+        <v/>
+      </c>
+      <c r="L70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v/>
       </c>
-      <c r="M59" s="125" t="str">
+      <c r="M70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v/>
       </c>
-      <c r="N59" s="125" t="str">
+      <c r="N70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*Betas_Per_Segment[[#This Row],[Allocated debt]]/Betas_Per_Segment[[#This Row],[Scaled estimated equity ]]),"")</f>
         <v/>
       </c>
-      <c r="O59" s="125" t="str">
+      <c r="O70" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="P59" s="125" t="str">
+      <c r="P70" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v/>
       </c>
-      <c r="Q59" s="72" t="str">
+      <c r="Q70" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="S59" s="166" t="s">
+      <c r="S70" s="170" t="s">
         <v>460</v>
       </c>
-      <c r="T59" s="166"/>
-      <c r="U59" s="166"/>
-      <c r="V59" s="166"/>
-      <c r="W59" s="166"/>
-      <c r="X59" s="166"/>
-    </row>
-    <row r="60" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C60" s="148" t="str">
+      <c r="T70" s="170"/>
+      <c r="U70" s="170"/>
+      <c r="V70" s="170"/>
+      <c r="W70" s="170"/>
+      <c r="X70" s="170"/>
+    </row>
+    <row r="71" spans="2:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C71" s="148" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D60" s="154" t="str">
+      <c r="D71" s="154" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],3,FALSE)),3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E60" s="72" t="str">
+      <c r="E71" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F60" s="138" t="str">
+      <c r="F71" s="138" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]/Estimated_Firm_Value,"")</f>
         <v/>
       </c>
-      <c r="G60" s="125" t="str">
+      <c r="G71" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),8,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H60" s="72" t="str">
+      <c r="H71" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="I60" s="125" t="str">
+      <c r="I71" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v/>
       </c>
-      <c r="J60" s="125" t="str">
+      <c r="J71" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated debt]]/SUM(Betas_Per_Segment[Estimated debt])*Company_Debt,"")</f>
         <v/>
       </c>
-      <c r="K60" s="125" t="str">
-        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$51,"")</f>
-        <v/>
-      </c>
-      <c r="L60" s="125" t="str">
+      <c r="K71" s="125" t="str">
+        <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]*Betas_Per_Segment[Industry D/E]/$F$62,"")</f>
+        <v/>
+      </c>
+      <c r="L71" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated Value]]-Betas_Per_Segment[[#This Row],[Allocated debt]],"")</f>
         <v/>
       </c>
-      <c r="M60" s="125" t="str">
+      <c r="M71" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated equity]]/SUM(Betas_Per_Segment[Estimated equity])*Company_Equity,"")</f>
         <v/>
       </c>
-      <c r="N60" s="125"/>
-      <c r="O60" s="125" t="str">
+      <c r="N71" s="125"/>
+      <c r="O71" s="125" t="str">
         <f ca="1">IFERROR(VLOOKUP(Betas_Per_Segment[[#This Row],[Segment]],INDIRECT(VLOOKUP(Industry_Average,Industry_TableConverter[],2,FALSE)),4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="P60" s="125" t="str">
+      <c r="P71" s="125" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment[[#This Row],[Estimated levered beta using debt allocation]],"")</f>
         <v/>
       </c>
-      <c r="Q60" s="72" t="str">
+      <c r="Q71" s="72" t="str">
         <f ca="1">IFERROR(Betas_Per_Segment[[#This Row],[Estimated levered beta]]*Betas_Per_Segment[[#This Row],[Firm Value Proportion]],"")</f>
         <v/>
       </c>
-      <c r="S60" s="166"/>
-      <c r="T60" s="166"/>
-      <c r="U60" s="166"/>
-      <c r="V60" s="166"/>
-      <c r="W60" s="166"/>
-      <c r="X60" s="166"/>
-    </row>
-    <row r="61" spans="2:24" ht="23.25" customHeight="1" thickTop="1">
-      <c r="C61" s="151" t="s">
+      <c r="S71" s="170"/>
+      <c r="T71" s="170"/>
+      <c r="U71" s="170"/>
+      <c r="V71" s="170"/>
+      <c r="W71" s="170"/>
+      <c r="X71" s="170"/>
+    </row>
+    <row r="72" spans="2:24" ht="23.25" customHeight="1" thickTop="1">
+      <c r="C72" s="151" t="s">
         <v>302</v>
       </c>
-      <c r="D61" s="151"/>
-      <c r="E61" s="151">
+      <c r="D72" s="151"/>
+      <c r="E72" s="151">
         <f ca="1">SUBTOTAL(109,Betas_Per_Segment[Estimated Value])</f>
         <v>174590.94103304454</v>
       </c>
-      <c r="F61" s="151"/>
-      <c r="G61" s="161">
+      <c r="F72" s="151"/>
+      <c r="G72" s="161">
         <f ca="1">SUM(Betas_Per_Segment[Firm value proportion * Unlevered Beta])</f>
         <v>0.92070493947431598</v>
       </c>
-      <c r="H61" s="151"/>
-      <c r="I61" s="161">
+      <c r="H72" s="151"/>
+      <c r="I72" s="161">
         <f ca="1">SUM(Betas_Per_Segment[Firm value proportion * Levered Beta2])</f>
         <v>1.369548597468045</v>
       </c>
-      <c r="J61" s="161"/>
-      <c r="K61" s="161"/>
-      <c r="L61" s="161"/>
-      <c r="M61" s="161">
+      <c r="J72" s="161"/>
+      <c r="K72" s="161"/>
+      <c r="L72" s="161"/>
+      <c r="M72" s="161">
         <f ca="1">SUBTOTAL(109,Betas_Per_Segment[[Scaled estimated equity ]])</f>
         <v>9999.9999999999982</v>
       </c>
-      <c r="N61">
+      <c r="N72">
         <f ca="1">SUM(Betas_Per_Segment[Firm value proportion * Levered Beta debt])</f>
         <v>1.3605273792900041</v>
       </c>
-      <c r="O61">
+      <c r="O72">
         <f ca="1">SUM(Betas_Per_Segment[Industry D/E])</f>
         <v>1.6823012700021569</v>
       </c>
-      <c r="Q61" s="151"/>
-    </row>
-    <row r="63" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B63" t="s">
+      <c r="Q72" s="151"/>
+    </row>
+    <row r="74" spans="2:24" ht="15.75" thickBot="1">
+      <c r="B74" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="64" spans="2:24" ht="30.75" customHeight="1">
-      <c r="C64" s="160" t="s">
+    <row r="75" spans="2:24" ht="30.75" customHeight="1">
+      <c r="C75" s="160" t="s">
         <v>469</v>
       </c>
-      <c r="D64" s="40" t="s">
+      <c r="D75" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="E64" s="40" t="s">
+      <c r="E75" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="F64" s="40" t="s">
+      <c r="F75" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="G64" s="40" t="s">
+      <c r="G75" s="40" t="s">
         <v>301</v>
       </c>
-      <c r="H64" s="40" t="s">
+      <c r="H75" s="40" t="s">
         <v>443</v>
       </c>
-      <c r="I64" s="40" t="s">
+      <c r="I75" s="40" t="s">
         <v>457</v>
       </c>
-      <c r="J64" s="159" t="s">
+      <c r="J75" s="159" t="s">
         <v>477</v>
       </c>
-      <c r="K64" s="159" t="s">
+      <c r="K75" s="159" t="s">
         <v>478</v>
       </c>
-      <c r="L64" s="73" t="s">
+      <c r="L75" s="73" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="65" spans="3:12" ht="15.75" thickBot="1">
-      <c r="C65" s="150" t="str">
-        <f>IF(C40="","",C40)</f>
+    <row r="76" spans="2:24" ht="15.75" thickBot="1">
+      <c r="C76" s="150" t="str">
+        <f>IF(C51="","",C51)</f>
         <v>Metals &amp; Mining</v>
       </c>
-      <c r="D65" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E65" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F65" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G65" s="125">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+      <c r="D76" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E76" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F76" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G76" s="125">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
         <v>1.0806756987285682</v>
       </c>
-      <c r="H65" s="155" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I65" s="125">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+      <c r="H76" s="155" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I76" s="125">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>1.6075051018587452</v>
       </c>
-      <c r="J65" s="125"/>
-      <c r="K65" s="125"/>
-      <c r="L65" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C66" s="150" t="str">
-        <f t="shared" ref="C66:C71" si="1">IF(C41="","",C41)</f>
+      <c r="J76" s="125"/>
+      <c r="K76" s="125"/>
+      <c r="L76" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="2:24" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C77" s="150" t="str">
+        <f t="shared" ref="C77:C82" si="1">IF(C52="","",C52)</f>
         <v>Chemical (Diversified)</v>
       </c>
-      <c r="D66" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E66" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F66" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G66" s="125">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+      <c r="D77" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E77" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F77" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G77" s="125">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="H66" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I66" s="125">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+      <c r="H77" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I77" s="125">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>0</v>
       </c>
-      <c r="J66" s="125"/>
-      <c r="K66" s="125"/>
-      <c r="L66" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C67" s="150" t="str">
+      <c r="J77" s="125"/>
+      <c r="K77" s="125"/>
+      <c r="L77" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:24" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C78" s="150" t="str">
         <f t="shared" si="1"/>
         <v>Coal &amp; Related Energy</v>
       </c>
-      <c r="D67" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E67" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F67" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G67" s="125">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+      <c r="D78" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E78" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F78" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G78" s="125">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="H67" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I67" s="125">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+      <c r="H78" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I78" s="125">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
         <v>0</v>
       </c>
-      <c r="J67" s="125"/>
-      <c r="K67" s="125"/>
-      <c r="L67" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C68" s="150" t="str">
+      <c r="J78" s="125"/>
+      <c r="K78" s="125"/>
+      <c r="L78" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="2:24" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C79" s="150" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D68" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E68" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F68" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G68" s="125" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H68" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I68" s="125" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
-        <v/>
-      </c>
-      <c r="J68" s="125"/>
-      <c r="K68" s="125"/>
-      <c r="L68" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C69" s="150" t="str">
+      <c r="D79" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E79" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F79" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G79" s="125" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H79" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I79" s="125" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+        <v/>
+      </c>
+      <c r="J79" s="125"/>
+      <c r="K79" s="125"/>
+      <c r="L79" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="2:24" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C80" s="150" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D69" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E69" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F69" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G69" s="125" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H69" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I69" s="125" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
-        <v/>
-      </c>
-      <c r="J69" s="125"/>
-      <c r="K69" s="125"/>
-      <c r="L69" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C70" s="150" t="str">
+      <c r="D80" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E80" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F80" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G80" s="125" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H80" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I80" s="125" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+        <v/>
+      </c>
+      <c r="J80" s="125"/>
+      <c r="K80" s="125"/>
+      <c r="L80" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C81" s="150" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D70" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E70" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F70" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G70" s="125" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H70" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I70" s="125" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
-        <v/>
-      </c>
-      <c r="J70" s="125"/>
-      <c r="K70" s="125"/>
-      <c r="L70" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C71" s="150" t="str">
+      <c r="D81" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E81" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F81" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G81" s="125" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H81" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I81" s="125" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+        <v/>
+      </c>
+      <c r="J81" s="125"/>
+      <c r="K81" s="125"/>
+      <c r="L81" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="3:12" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C82" s="150" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D71" s="154" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="E71" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[EV/Sales]]*VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F71" s="144" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Estimated Value]]/Tabell28[[#Totals],[Estimated Value]],"")</f>
-        <v/>
-      </c>
-      <c r="G71" s="125" t="str">
-        <f>IFERROR(VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Tabell28[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Tabell28[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H71" s="156" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Unlevered beta]],"")</f>
-        <v/>
-      </c>
-      <c r="I71" s="125" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
-        <v/>
-      </c>
-      <c r="J71" s="125"/>
-      <c r="K71" s="125"/>
-      <c r="L71" s="72" t="str">
-        <f>IFERROR(Tabell28[[#This Row],[Firm Value Proportion]]*Tabell28[[#This Row],[Estimated levered beta]],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="3:12" ht="15.75" thickTop="1">
-      <c r="C72" s="5" t="s">
+      <c r="D82" s="154" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_US[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_China[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_Europe[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],EV_Sales_India[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E82" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[EV/Sales]]*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F82" s="144" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Estimated Value]]/Betas_Per_Segment_Region[[#Totals],[Estimated Value]],"")</f>
+        <v/>
+      </c>
+      <c r="G82" s="125" t="str">
+        <f>IFERROR(VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],3,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_US[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],4,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_China[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],5,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_Europe[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],6,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_India[],8,FALSE)+VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Operations_Per_Segment_Region[],7,FALSE)*VLOOKUP(Betas_Per_Segment_Region[[#This Row],[Segment]],Industry_Average_EmergingMarkets[],8,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H82" s="156" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Unlevered beta]],"")</f>
+        <v/>
+      </c>
+      <c r="I82" s="125" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Unlevered beta]]*(1+(1-Company_Tax_Rate)*(Company_Debt/Company_Equity)),"")</f>
+        <v/>
+      </c>
+      <c r="J82" s="125"/>
+      <c r="K82" s="125"/>
+      <c r="L82" s="72" t="str">
+        <f>IFERROR(Betas_Per_Segment_Region[[#This Row],[Firm Value Proportion]]*Betas_Per_Segment_Region[[#This Row],[Estimated levered beta]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="3:12" ht="15.75" thickTop="1">
+      <c r="C83" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="E72">
-        <f>SUM(Tabell28[Estimated Value])</f>
+      <c r="E83">
+        <f>SUM(Betas_Per_Segment_Region[Estimated Value])</f>
         <v>0</v>
       </c>
-      <c r="G72" s="158">
-        <f>SUM(Tabell28[Firm value proportion * Unlevered Beta])</f>
+      <c r="G83" s="158">
+        <f>SUM(Betas_Per_Segment_Region[Firm value proportion * Unlevered Beta])</f>
         <v>0</v>
       </c>
-      <c r="I72" s="158">
-        <f>SUM(Tabell28[Firm value proportion * Levered Beta])</f>
+      <c r="I83" s="158">
+        <f>SUM(Betas_Per_Segment_Region[Firm value proportion * Levered Beta])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="3:12" ht="135">
-      <c r="D73" s="40" t="s">
+    <row r="84" spans="3:12" ht="135">
+      <c r="D84" s="40" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="76" spans="3:12">
-      <c r="C76" s="47"/>
-    </row>
-    <row r="77" spans="3:12">
-      <c r="C77" s="47"/>
-    </row>
-    <row r="87" spans="2:4">
-      <c r="B87" t="s">
+    <row r="87" spans="3:12">
+      <c r="C87" s="47"/>
+    </row>
+    <row r="88" spans="3:12">
+      <c r="C88" s="47"/>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="88" spans="2:4">
-      <c r="C88" s="132" t="s">
+    <row r="99" spans="2:4">
+      <c r="C99" s="132" t="s">
         <v>427</v>
       </c>
-      <c r="D88" s="134">
+      <c r="D99" s="134">
         <v>0.35</v>
       </c>
     </row>
-    <row r="126" ht="30.75" customHeight="1"/>
+    <row r="137" ht="30.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="S59:X60"/>
-    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="S70:X71"/>
+    <mergeCell ref="E49:I49"/>
     <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C62:D62"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="R54:T55"/>
+    <mergeCell ref="R65:T66"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="decimal" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35">
+  <dataValidations count="3">
+    <dataValidation type="decimal" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46">
       <formula1>100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C57">
       <formula1>Input_Industries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8">
+      <formula1>Input_Company_Types</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -8225,7 +8455,7 @@
           <x14:formula1>
             <xm:f>'Input data &amp; validation'!$B$20:$B$25</xm:f>
           </x14:formula1>
-          <xm:sqref>C51:D51</xm:sqref>
+          <xm:sqref>C62:D62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8237,8 +8467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView showGridLines="0" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8260,12 +8490,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="3" spans="2:16" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="25" t="s">
@@ -8289,17 +8519,17 @@
       <c r="P3" s="22"/>
     </row>
     <row r="4" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="2:16" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="24.95" customHeight="1">
-      <c r="C7" s="173" t="s">
+      <c r="C7" s="177" t="s">
         <v>262</v>
       </c>
-      <c r="D7" s="173"/>
-      <c r="E7" s="173"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
     </row>
     <row r="8" spans="2:16">
       <c r="E8" s="45" t="s">
@@ -8310,12 +8540,12 @@
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B20" s="164" t="s">
+      <c r="B20" s="168" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B21" s="164"/>
+      <c r="B21" s="168"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="25" t="s">
@@ -8333,7 +8563,7 @@
       <c r="P21" s="22"/>
     </row>
     <row r="22" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B22" s="164"/>
+      <c r="B22" s="168"/>
     </row>
     <row r="23" spans="2:16" ht="7.5" customHeight="1">
       <c r="B23" s="1"/>
@@ -8386,12 +8616,12 @@
       <c r="B35" s="1"/>
     </row>
     <row r="36" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B36" s="164" t="s">
+      <c r="B36" s="168" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="37" spans="2:16" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B37" s="164"/>
+      <c r="B37" s="168"/>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="25" t="s">
@@ -8409,7 +8639,7 @@
       <c r="P37" s="22"/>
     </row>
     <row r="38" spans="2:16" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B38" s="164"/>
+      <c r="B38" s="168"/>
     </row>
     <row r="39" spans="2:16" ht="7.5" customHeight="1">
       <c r="B39" s="1"/>
@@ -8498,8 +8728,8 @@
       <c r="H52" s="38"/>
     </row>
     <row r="53" spans="4:8">
-      <c r="F53" s="172"/>
-      <c r="G53" s="172"/>
+      <c r="F53" s="176"/>
+      <c r="G53" s="176"/>
       <c r="H53" s="38"/>
     </row>
     <row r="54" spans="4:8">
@@ -8718,7 +8948,7 @@
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="B36:B38"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65">
       <formula1>100</formula1>
     </dataValidation>
@@ -8766,12 +8996,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="180" t="s">
+      <c r="B2" s="184" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="180"/>
+      <c r="B3" s="184"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -8794,28 +9024,28 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="180"/>
+      <c r="B4" s="184"/>
     </row>
     <row r="5" spans="2:14" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="174" t="s">
+      <c r="B7" s="178" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="174"/>
-      <c r="D7" s="174"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
       <c r="E7" t="s">
         <v>281</v>
       </c>
       <c r="H7" s="34"/>
     </row>
     <row r="8" spans="2:14" ht="27.75" customHeight="1">
-      <c r="B8" s="175" t="s">
+      <c r="B8" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="176"/>
-      <c r="D8" s="177"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
       <c r="E8" s="54">
         <v>0.67</v>
       </c>
@@ -8826,18 +9056,18 @@
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="181" t="s">
+      <c r="B11" s="185" t="s">
         <v>267</v>
       </c>
-      <c r="C11" s="181"/>
-      <c r="D11" s="179" t="s">
+      <c r="C11" s="185"/>
+      <c r="D11" s="183" t="s">
         <v>273</v>
       </c>
-      <c r="E11" s="179"/>
-      <c r="G11" s="178" t="s">
+      <c r="E11" s="183"/>
+      <c r="G11" s="182" t="s">
         <v>277</v>
       </c>
-      <c r="H11" s="178"/>
+      <c r="H11" s="182"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="35" t="s">
@@ -8975,20 +9205,20 @@
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="174" t="s">
+      <c r="B18" s="178" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="174"/>
-      <c r="D18" s="174"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="178"/>
       <c r="E18" t="s">
         <v>281</v>
       </c>
       <c r="F18" s="50"/>
     </row>
     <row r="19" spans="2:6" ht="31.5">
-      <c r="B19" s="175"/>
-      <c r="C19" s="176"/>
-      <c r="D19" s="177"/>
+      <c r="B19" s="179"/>
+      <c r="C19" s="180"/>
+      <c r="D19" s="181"/>
       <c r="E19" s="54">
         <v>0.67</v>
       </c>
@@ -9071,12 +9301,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -9099,7 +9329,7 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="1:14" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
@@ -11681,10 +11911,10 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="30" customHeight="1">
-      <c r="A108" s="182" t="s">
+      <c r="A108" s="186" t="s">
         <v>420</v>
       </c>
-      <c r="B108" s="182"/>
+      <c r="B108" s="186"/>
     </row>
     <row r="109" spans="1:9">
       <c r="B109" s="90" t="s">
@@ -14235,10 +14465,10 @@
       </c>
     </row>
     <row r="208" spans="1:9" ht="30" customHeight="1">
-      <c r="A208" s="182" t="s">
+      <c r="A208" s="186" t="s">
         <v>415</v>
       </c>
-      <c r="B208" s="182"/>
+      <c r="B208" s="186"/>
     </row>
     <row r="209" spans="2:9">
       <c r="B209" s="90" t="s">
@@ -16763,11 +16993,11 @@
       </c>
     </row>
     <row r="307" spans="1:9" ht="30" customHeight="1">
-      <c r="A307" s="183" t="s">
+      <c r="A307" s="187" t="s">
         <v>408</v>
       </c>
-      <c r="B307" s="183"/>
-      <c r="C307" s="183"/>
+      <c r="B307" s="187"/>
+      <c r="C307" s="187"/>
     </row>
     <row r="308" spans="1:9">
       <c r="B308" s="90" t="s">
@@ -19292,10 +19522,10 @@
       </c>
     </row>
     <row r="406" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A406" s="182" t="s">
+      <c r="A406" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="B406" s="182"/>
+      <c r="B406" s="186"/>
     </row>
     <row r="407" spans="1:9">
       <c r="B407" s="90" t="s">
@@ -21768,10 +21998,10 @@
       </c>
     </row>
     <row r="503" spans="1:9" ht="28.5" customHeight="1">
-      <c r="A503" s="182" t="s">
+      <c r="A503" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="B503" s="182"/>
+      <c r="B503" s="186"/>
     </row>
     <row r="504" spans="1:9">
       <c r="B504" s="90" t="s">
@@ -24088,18 +24318,18 @@
       </c>
     </row>
     <row r="594" spans="1:16" ht="34.5" customHeight="1">
-      <c r="A594" s="182" t="s">
+      <c r="A594" s="186" t="s">
         <v>431</v>
       </c>
-      <c r="B594" s="182"/>
-      <c r="C594" s="182"/>
+      <c r="B594" s="186"/>
+      <c r="C594" s="186"/>
     </row>
     <row r="595" spans="1:16" ht="15.75" thickBot="1">
-      <c r="B595" s="172" t="s">
+      <c r="B595" s="176" t="s">
         <v>435</v>
       </c>
-      <c r="C595" s="172"/>
-      <c r="D595" s="172"/>
+      <c r="C595" s="176"/>
+      <c r="D595" s="176"/>
       <c r="F595" t="s">
         <v>282</v>
       </c>
@@ -28489,12 +28719,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:39" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="3" spans="2:39" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -28517,7 +28747,7 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:39" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="2:39" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
@@ -36018,15 +36248,15 @@
       <c r="E137" s="9"/>
     </row>
     <row r="138" spans="2:24">
-      <c r="C138" s="184" t="s">
+      <c r="C138" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D138" s="184"/>
-      <c r="E138" s="185" t="s">
+      <c r="D138" s="188"/>
+      <c r="E138" s="189" t="s">
         <v>287</v>
       </c>
-      <c r="F138" s="185"/>
-      <c r="G138" s="185"/>
+      <c r="F138" s="189"/>
+      <c r="G138" s="189"/>
     </row>
     <row r="139" spans="2:24" ht="33" customHeight="1">
       <c r="B139" s="62" t="s">
@@ -36304,13 +36534,13 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad7"/>
-  <dimension ref="B1:N157"/>
+  <dimension ref="B1:Q157"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="D141" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="H142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H143" sqref="H143"/>
+      <selection pane="bottomRight" activeCell="R144" sqref="R144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36323,6 +36553,7 @@
     <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
     <col min="17" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36330,12 +36561,12 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="168" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="164"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="23"/>
       <c r="D3" s="25" t="s">
         <v>206</v>
@@ -36358,27 +36589,27 @@
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:14" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="164"/>
+      <c r="B4" s="168"/>
     </row>
     <row r="5" spans="2:14" ht="7.5" customHeight="1">
       <c r="B5" s="1"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172"/>
-      <c r="F7" s="172" t="s">
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="F7" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="172"/>
-      <c r="H7" s="172"/>
-      <c r="J7" s="172" t="s">
+      <c r="G7" s="176"/>
+      <c r="H7" s="176"/>
+      <c r="J7" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="172"/>
-      <c r="L7" s="172"/>
+      <c r="K7" s="176"/>
+      <c r="L7" s="176"/>
     </row>
     <row r="8" spans="2:14">
       <c r="B8" t="s">
@@ -39691,7 +39922,7 @@
         <v>41325</v>
       </c>
     </row>
-    <row r="129" spans="2:12">
+    <row r="129" spans="2:17">
       <c r="B129" t="s">
         <v>164</v>
       </c>
@@ -39702,7 +39933,7 @@
         <v>41360</v>
       </c>
     </row>
-    <row r="130" spans="2:12">
+    <row r="130" spans="2:17">
       <c r="B130" t="s">
         <v>165</v>
       </c>
@@ -39713,7 +39944,7 @@
         <v>40876</v>
       </c>
     </row>
-    <row r="131" spans="2:12">
+    <row r="131" spans="2:17">
       <c r="B131" t="s">
         <v>166</v>
       </c>
@@ -39724,7 +39955,7 @@
         <v>41634</v>
       </c>
     </row>
-    <row r="132" spans="2:12">
+    <row r="132" spans="2:17">
       <c r="B132" t="s">
         <v>167</v>
       </c>
@@ -39735,7 +39966,7 @@
         <v>41012</v>
       </c>
     </row>
-    <row r="133" spans="2:12">
+    <row r="133" spans="2:17">
       <c r="B133" t="s">
         <v>168</v>
       </c>
@@ -39746,7 +39977,7 @@
         <v>41435</v>
       </c>
     </row>
-    <row r="134" spans="2:12">
+    <row r="134" spans="2:17">
       <c r="B134" t="s">
         <v>169</v>
       </c>
@@ -39757,7 +39988,7 @@
         <v>41002</v>
       </c>
     </row>
-    <row r="135" spans="2:12">
+    <row r="135" spans="2:17">
       <c r="B135" t="s">
         <v>170</v>
       </c>
@@ -39768,7 +39999,7 @@
         <v>41442</v>
       </c>
     </row>
-    <row r="136" spans="2:12">
+    <row r="136" spans="2:17">
       <c r="B136" t="s">
         <v>171</v>
       </c>
@@ -39779,7 +40010,7 @@
         <v>41779</v>
       </c>
     </row>
-    <row r="137" spans="2:12">
+    <row r="137" spans="2:17">
       <c r="B137" t="s">
         <v>172</v>
       </c>
@@ -39790,44 +40021,62 @@
         <v>40876</v>
       </c>
     </row>
-    <row r="141" spans="2:12">
+    <row r="141" spans="2:17">
       <c r="B141" t="s">
+        <v>506</v>
+      </c>
+      <c r="H141" t="s">
+        <v>507</v>
+      </c>
+      <c r="N141" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="142" spans="2:17">
+      <c r="B142" t="s">
+        <v>486</v>
+      </c>
+      <c r="C142" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="142" spans="2:12">
-      <c r="B142" t="s">
+      <c r="D142" t="s">
+        <v>489</v>
+      </c>
+      <c r="E142" t="s">
+        <v>490</v>
+      </c>
+      <c r="F142" t="s">
         <v>488</v>
       </c>
-      <c r="C142" t="s">
+      <c r="H142" t="s">
+        <v>497</v>
+      </c>
+      <c r="I142" t="s">
+        <v>487</v>
+      </c>
+      <c r="J142" t="s">
         <v>489</v>
       </c>
-      <c r="D142" t="s">
-        <v>491</v>
-      </c>
-      <c r="E142" t="s">
-        <v>492</v>
-      </c>
-      <c r="F142" t="s">
+      <c r="K142" t="s">
         <v>490</v>
       </c>
-      <c r="H142" t="s">
-        <v>499</v>
-      </c>
-      <c r="I142" t="s">
-        <v>489</v>
-      </c>
-      <c r="J142" t="s">
-        <v>491</v>
-      </c>
-      <c r="K142" t="s">
-        <v>492</v>
-      </c>
       <c r="L142" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="143" spans="2:12">
+        <v>488</v>
+      </c>
+      <c r="N142" t="s">
+        <v>508</v>
+      </c>
+      <c r="O142" t="s">
+        <v>487</v>
+      </c>
+      <c r="P142" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="143" spans="2:17">
       <c r="B143">
         <v>8.5</v>
       </c>
@@ -39858,8 +40107,20 @@
       <c r="L143" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="144" spans="2:12">
+      <c r="N143">
+        <v>3</v>
+      </c>
+      <c r="O143">
+        <v>100000</v>
+      </c>
+      <c r="P143" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q143">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="2:17">
       <c r="B144">
         <v>6.5</v>
       </c>
@@ -39892,8 +40153,20 @@
       <c r="L144" s="21">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="145" spans="2:12">
+      <c r="N144">
+        <v>2.5</v>
+      </c>
+      <c r="O144">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="P144" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q144">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17">
       <c r="B145">
         <v>5.5</v>
       </c>
@@ -39926,8 +40199,20 @@
       <c r="L145" s="21">
         <v>8.5000000000000006E-3</v>
       </c>
-    </row>
-    <row r="146" spans="2:12">
+      <c r="N145">
+        <v>2</v>
+      </c>
+      <c r="O145">
+        <v>2.4999899999999999</v>
+      </c>
+      <c r="P145" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q145">
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="2:17">
       <c r="B146">
         <v>4.25</v>
       </c>
@@ -39960,8 +40245,20 @@
       <c r="L146" s="21">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="147" spans="2:12">
+      <c r="N146">
+        <v>1.5</v>
+      </c>
+      <c r="O146">
+        <v>1.9999899999999999</v>
+      </c>
+      <c r="P146" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q146">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17">
       <c r="B147">
         <v>3</v>
       </c>
@@ -39994,8 +40291,20 @@
       <c r="L147" s="21">
         <v>1.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="148" spans="2:12">
+      <c r="N147">
+        <v>1.2</v>
+      </c>
+      <c r="O147">
+        <v>1.4999899999999999</v>
+      </c>
+      <c r="P147" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q147">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="2:17">
       <c r="B148">
         <v>2.5</v>
       </c>
@@ -40028,8 +40337,20 @@
       <c r="L148" s="21">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="149" spans="2:12">
+      <c r="N148">
+        <v>0.9</v>
+      </c>
+      <c r="O148">
+        <v>1.199999</v>
+      </c>
+      <c r="P148" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q148">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17">
       <c r="B149">
         <v>2.25</v>
       </c>
@@ -40062,8 +40383,20 @@
       <c r="L149" s="21">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="150" spans="2:12">
+      <c r="N149">
+        <v>0.75</v>
+      </c>
+      <c r="O149">
+        <v>0.89999899999999999</v>
+      </c>
+      <c r="P149" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q149">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="150" spans="2:17">
       <c r="B150">
         <v>2</v>
       </c>
@@ -40096,8 +40429,20 @@
       <c r="L150" s="21">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="151" spans="2:12">
+      <c r="N150">
+        <v>0.6</v>
+      </c>
+      <c r="O150">
+        <v>0.74999899999999997</v>
+      </c>
+      <c r="P150" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q150">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="151" spans="2:17">
       <c r="B151">
         <v>1.75</v>
       </c>
@@ -40130,8 +40475,20 @@
       <c r="L151" s="21">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="152" spans="2:12">
+      <c r="N151">
+        <v>0.5</v>
+      </c>
+      <c r="O151">
+        <v>0.59999899999999995</v>
+      </c>
+      <c r="P151" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q151">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="2:17">
       <c r="B152">
         <v>1.5</v>
       </c>
@@ -40164,8 +40521,20 @@
       <c r="L152" s="21">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="153" spans="2:12">
+      <c r="N152">
+        <v>0.4</v>
+      </c>
+      <c r="O152">
+        <v>0.49999900000000003</v>
+      </c>
+      <c r="P152" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q152">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17">
       <c r="B153">
         <v>1.25</v>
       </c>
@@ -40198,8 +40567,20 @@
       <c r="L153" s="21">
         <v>7.2499999999999995E-2</v>
       </c>
-    </row>
-    <row r="154" spans="2:12">
+      <c r="N153">
+        <v>0.3</v>
+      </c>
+      <c r="O153">
+        <v>0.39999899999999999</v>
+      </c>
+      <c r="P153" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q153">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="2:17">
       <c r="B154">
         <v>0.8</v>
       </c>
@@ -40232,8 +40613,20 @@
       <c r="L154" s="21">
         <v>8.7499999999999994E-2</v>
       </c>
-    </row>
-    <row r="155" spans="2:12">
+      <c r="N154">
+        <v>0.2</v>
+      </c>
+      <c r="O154">
+        <v>0.29999900000000002</v>
+      </c>
+      <c r="P154" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q154">
+        <v>8.7499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="2:17">
       <c r="B155">
         <v>0.65</v>
       </c>
@@ -40242,10 +40635,10 @@
         <v>0.79999900000000002</v>
       </c>
       <c r="D155" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E155" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F155" s="21">
         <v>9.5000000000000001E-2</v>
@@ -40258,16 +40651,28 @@
         <v>1.2499990000000001</v>
       </c>
       <c r="J155" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K155" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L155" s="21">
         <v>9.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="156" spans="2:12">
+      <c r="N155">
+        <v>0.1</v>
+      </c>
+      <c r="O155">
+        <v>0.19999900000000001</v>
+      </c>
+      <c r="P155" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q155">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="2:17">
       <c r="B156">
         <v>0.2</v>
       </c>
@@ -40276,10 +40681,10 @@
         <v>0.64999899999999999</v>
       </c>
       <c r="D156" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E156" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F156" s="21">
         <v>0.105</v>
@@ -40292,16 +40697,28 @@
         <v>0.79999900000000002</v>
       </c>
       <c r="J156" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K156" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="L156" s="21">
         <v>0.105</v>
       </c>
-    </row>
-    <row r="157" spans="2:12">
+      <c r="N156">
+        <v>0.05</v>
+      </c>
+      <c r="O156">
+        <v>9.9999000000000005E-2</v>
+      </c>
+      <c r="P156" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q156">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="157" spans="2:17">
       <c r="B157">
         <v>-100000</v>
       </c>
@@ -40310,10 +40727,10 @@
         <v>0.19999900000000001</v>
       </c>
       <c r="D157" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E157" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F157" s="21">
         <v>0.12</v>
@@ -40326,12 +40743,24 @@
         <v>0.49999900000000003</v>
       </c>
       <c r="J157" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="K157" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="L157" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="N157">
+        <v>-100000</v>
+      </c>
+      <c r="O157">
+        <v>4.9999000000000002E-2</v>
+      </c>
+      <c r="P157" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q157">
         <v>0.12</v>
       </c>
     </row>
@@ -40349,12 +40778,13 @@
     <hyperlink ref="E3" location="'Models &amp; inputs'!B3" display="Models &amp;  inputs"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -40363,8 +40793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B25"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40386,13 +40816,13 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="2:15" s="2" customFormat="1" ht="9.75" customHeight="1">
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="190" t="s">
         <v>234</v>
       </c>
       <c r="C2" s="68"/>
     </row>
     <row r="3" spans="2:15" s="2" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="B3" s="186"/>
+      <c r="B3" s="190"/>
       <c r="C3" s="68"/>
       <c r="D3" s="23"/>
       <c r="E3" s="25" t="s">
@@ -40416,7 +40846,7 @@
       <c r="O3" s="22"/>
     </row>
     <row r="4" spans="2:15" s="2" customFormat="1" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B4" s="186"/>
+      <c r="B4" s="190"/>
       <c r="C4" s="68"/>
     </row>
     <row r="5" spans="2:15" ht="7.5" customHeight="1">
@@ -40436,6 +40866,12 @@
       <c r="G7" t="s">
         <v>297</v>
       </c>
+      <c r="I7" t="s">
+        <v>520</v>
+      </c>
+      <c r="J7" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="8" spans="2:15" ht="15.75">
       <c r="B8" t="s">
@@ -40447,6 +40883,12 @@
       <c r="G8" s="75" t="s">
         <v>320</v>
       </c>
+      <c r="I8" t="s">
+        <v>522</v>
+      </c>
+      <c r="J8" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="9" spans="2:15" ht="15.75">
       <c r="B9" t="s">
@@ -40461,6 +40903,12 @@
       <c r="G9" s="75" t="s">
         <v>321</v>
       </c>
+      <c r="I9" t="s">
+        <v>521</v>
+      </c>
+      <c r="J9" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="10" spans="2:15" ht="15.75">
       <c r="B10" t="s">
@@ -40468,6 +40916,12 @@
       </c>
       <c r="G10" s="75" t="s">
         <v>322</v>
+      </c>
+      <c r="I10" t="s">
+        <v>527</v>
+      </c>
+      <c r="J10" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75">
@@ -40978,12 +41432,13 @@
     <hyperlink ref="F3" location="'Models &amp; inputs'!B3" display="Models &amp;  inputs"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>